<commit_message>
+ keyword table and table description table in metadata doc updates in eml creation process
</commit_message>
<xml_diff>
--- a/4.project.XX/Metadata.xlsx
+++ b/4.project.XX/Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargas/padl/longley-wood-spatial-data/4.project.110/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camilavargas/padl/template-repo/4.project.XX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBC83A7-4F53-A545-A939-8209D46C6A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E96BF3C-ADBD-9D48-84E4-974ACDAF4074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2104" uniqueCount="1151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2137" uniqueCount="1176">
   <si>
     <t>csv_E</t>
   </si>
@@ -3927,6 +3927,81 @@
   </si>
   <si>
     <t>Wildlife Conservation Society Climate Adaptation Fund</t>
+  </si>
+  <si>
+    <t>asguerra</t>
+  </si>
+  <si>
+    <t>Ana Sofia</t>
+  </si>
+  <si>
+    <t>Guerra</t>
+  </si>
+  <si>
+    <t>asg@ucsb.edu</t>
+  </si>
+  <si>
+    <t>jcaselle</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>Caselle</t>
+  </si>
+  <si>
+    <t>caselle@ucsb.edu</t>
+  </si>
+  <si>
+    <t>dmcc</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>McCauley</t>
+  </si>
+  <si>
+    <t>dmccauley@ucsb.edu</t>
+  </si>
+  <si>
+    <t>ejahn</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Jahn</t>
+  </si>
+  <si>
+    <t>mmorse</t>
+  </si>
+  <si>
+    <t>Marisa</t>
+  </si>
+  <si>
+    <t>Morse</t>
+  </si>
+  <si>
+    <t>kdavis</t>
+  </si>
+  <si>
+    <t>Kathryn</t>
+  </si>
+  <si>
+    <t>kmunsterman</t>
+  </si>
+  <si>
+    <t>Katrina</t>
+  </si>
+  <si>
+    <t>Munsterman</t>
+  </si>
+  <si>
+    <t>University of Michigan</t>
   </si>
 </sst>
 </file>
@@ -3937,7 +4012,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -3980,17 +4055,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Docs-Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="DejaVu Sans"/>
@@ -3999,6 +4063,31 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -4023,7 +4112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4035,11 +4124,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4323,7 +4415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -4391,7 +4483,7 @@
       <c r="F2">
         <v>2019</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="11">
         <v>44566</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -12668,7 +12760,7 @@
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>1098</v>
       </c>
       <c r="D2" t="s">
@@ -12687,7 +12779,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>1099</v>
       </c>
       <c r="D3" t="s">
@@ -12706,7 +12798,7 @@
       <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>1100</v>
       </c>
       <c r="D4" t="s">
@@ -12725,7 +12817,7 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>1101</v>
       </c>
       <c r="D5" t="s">
@@ -12746,7 +12838,7 @@
       <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>1102</v>
       </c>
       <c r="D6" t="s">
@@ -12767,7 +12859,7 @@
       <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="12" t="s">
         <v>1103</v>
       </c>
       <c r="D7" t="s">
@@ -12786,7 +12878,7 @@
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="12" t="s">
         <v>146</v>
       </c>
       <c r="D8" t="s">
@@ -12805,7 +12897,7 @@
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>1104</v>
       </c>
       <c r="D9" t="s">
@@ -12826,7 +12918,7 @@
       <c r="B10" s="1">
         <v>2</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>1105</v>
       </c>
       <c r="D10" t="s">
@@ -12847,7 +12939,7 @@
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="12" t="s">
         <v>1106</v>
       </c>
       <c r="D11" t="s">
@@ -12866,7 +12958,7 @@
       <c r="B12" s="1">
         <v>2</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>1107</v>
       </c>
       <c r="D12" t="s">
@@ -12885,7 +12977,7 @@
       <c r="B13" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>1108</v>
       </c>
       <c r="D13" t="s">
@@ -12904,7 +12996,7 @@
       <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>1109</v>
       </c>
       <c r="D14" t="s">
@@ -12925,7 +13017,7 @@
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="12" t="s">
         <v>1110</v>
       </c>
       <c r="D15" t="s">
@@ -12944,7 +13036,7 @@
       <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>1111</v>
       </c>
       <c r="D16" t="s">
@@ -12965,7 +13057,7 @@
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>1112</v>
       </c>
       <c r="D17" t="s">
@@ -13101,7 +13193,7 @@
       <c r="D5" t="s">
         <v>1116</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="13" t="s">
         <v>1127</v>
       </c>
     </row>
@@ -13486,10 +13578,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:N9"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -13505,7 +13597,7 @@
     <col min="14" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>1001</v>
       </c>
@@ -13549,221 +13641,429 @@
         <v>839</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" t="s">
+    <row r="2" spans="1:16">
+      <c r="A2" s="10" t="s">
         <v>1032</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>1033</v>
       </c>
-      <c r="C2"/>
-      <c r="D2" s="11" t="s">
+      <c r="C2" s="10"/>
+      <c r="D2" s="14" t="s">
         <v>1034</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="10" t="s">
         <v>1035</v>
       </c>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2" s="12" t="s">
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="15" t="s">
         <v>1036</v>
       </c>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="10" t="s">
         <v>1037</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="15" t="s">
         <v>1038</v>
       </c>
-      <c r="C3"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="15" t="s">
         <v>1039</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="10" t="s">
         <v>1035</v>
       </c>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
-      <c r="K3"/>
-      <c r="L3"/>
-      <c r="M3" s="12" t="s">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="15" t="s">
         <v>1040</v>
       </c>
-      <c r="N3"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
+      <c r="N3" s="15"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="10" t="s">
         <v>1041</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="15" t="s">
         <v>1042</v>
       </c>
-      <c r="C4"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="15" t="s">
         <v>1043</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>1044</v>
       </c>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
-      <c r="K4"/>
-      <c r="L4"/>
-      <c r="M4" t="s">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10" t="s">
         <v>1045</v>
       </c>
-      <c r="N4"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="10" t="s">
         <v>1046</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="15" t="s">
         <v>1047</v>
       </c>
-      <c r="C5"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="15" t="s">
         <v>1048</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="10" t="s">
         <v>1049</v>
       </c>
-      <c r="F5"/>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
-      <c r="K5"/>
-      <c r="L5"/>
-      <c r="M5"/>
-      <c r="N5"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" t="s">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="10" t="s">
         <v>1050</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>1051</v>
       </c>
-      <c r="C6"/>
-      <c r="D6" t="s">
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
         <v>1052</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="15" t="s">
         <v>1053</v>
       </c>
-      <c r="F6"/>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6" s="12" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="15" t="s">
         <v>1054</v>
       </c>
-      <c r="N6"/>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7" t="s">
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="10" t="s">
         <v>1030</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>1055</v>
       </c>
-      <c r="C7"/>
-      <c r="D7" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10" t="s">
         <v>1056</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="10" t="s">
         <v>1057</v>
       </c>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10" t="s">
         <v>1058</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>1059</v>
       </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8" t="s">
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="10" t="s">
         <v>1060</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>1061</v>
       </c>
-      <c r="C8"/>
-      <c r="D8" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="10" t="s">
         <v>1062</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="10" t="s">
         <v>1057</v>
       </c>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10" t="s">
         <v>1063</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="10" t="s">
         <v>1064</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9" t="s">
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="10" t="s">
         <v>1065</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>1066</v>
       </c>
-      <c r="C9"/>
-      <c r="D9" t="s">
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
         <v>1067</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="10" t="s">
         <v>1068</v>
       </c>
-      <c r="F9"/>
-      <c r="G9"/>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9" t="s">
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10" t="s">
         <v>1069</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="10" t="s">
         <v>1070</v>
       </c>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="10" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10" t="s">
+        <v>1154</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="10" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
+        <v>1159</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="10" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10" t="s">
+        <v>1163</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" ht="16">
+      <c r="A13" s="10" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="18" t="s">
+        <v>1166</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+    </row>
+    <row r="14" spans="1:16" ht="16">
+      <c r="A14" s="10" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C14" s="10"/>
+      <c r="D14" s="18" t="s">
+        <v>1169</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+    </row>
+    <row r="15" spans="1:16" ht="16">
+      <c r="A15" s="10" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C15" s="10"/>
+      <c r="D15" s="18" t="s">
+        <v>1048</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>1035</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+    </row>
+    <row r="16" spans="1:16" ht="16">
+      <c r="A16" s="10" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C16" s="10"/>
+      <c r="D16" s="18" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>1175</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N7" r:id="rId1" xr:uid="{6D8E9B07-68A5-B744-8C53-F7C1A0C65BFD}"/>
+    <hyperlink ref="N7" r:id="rId1" xr:uid="{94A6757E-AD30-BC4A-89EC-B34B6820E56B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>